<commit_message>
Casos de uso narrativos - Administrar Personal
Adjunto los 5 CDUN del Administrar personal y una actualización del CDU
Administrar Personal donde le quite un caso de uso para porque se podía
explicar en el narrativo.
</commit_message>
<xml_diff>
--- a/análisis/Casos de Uso Narrativos/CDUN - (Administrar Personal) Agregar Hostel Worker.xlsx
+++ b/análisis/Casos de Uso Narrativos/CDUN - (Administrar Personal) Agregar Hostel Worker.xlsx
@@ -517,7 +517,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
   <si>
     <t>Caso de uso</t>
   </si>
@@ -597,12 +597,6 @@
     <t>Roberto Cordero</t>
   </si>
   <si>
-    <t>Hostel Worker no agregado anteriormente</t>
-  </si>
-  <si>
-    <t>Hostel Worker agregado correctamente</t>
-  </si>
-  <si>
     <t>1.0</t>
   </si>
   <si>
@@ -630,28 +624,40 @@
     <t>????</t>
   </si>
   <si>
-    <t>El usuario ingresa los datos personales del  Hostel Worker.</t>
-  </si>
-  <si>
     <t>El usuario ingresa los un nombre de usuario y contraseña para el HostelWorker</t>
   </si>
   <si>
-    <t>El usuario es ingresado al sistema.</t>
-  </si>
-  <si>
-    <t>Fin del caso de uso.</t>
-  </si>
-  <si>
-    <t>1a</t>
-  </si>
-  <si>
     <t>El rut del Hostel Worker ya ha sido ingresado. Se indica el error y se pide ingresar un nuevo rut.</t>
   </si>
   <si>
-    <t>2a</t>
-  </si>
-  <si>
     <t>El nombre de usuario del Hostel Worker ya se encuentra usado. Se indica el error y se pide ingresar un nuevo nombre de usuario.</t>
+  </si>
+  <si>
+    <t>El caso de uso comienza cuando el administrador seleciona agregar Hostel Worker</t>
+  </si>
+  <si>
+    <t>El sistema valida los datos y los ingresa al sistema.</t>
+  </si>
+  <si>
+    <t>Fin del caso de uso</t>
+  </si>
+  <si>
+    <t>El sistema muestra un formulario para ingresar los datos.</t>
+  </si>
+  <si>
+    <t>5a</t>
+  </si>
+  <si>
+    <t>5b</t>
+  </si>
+  <si>
+    <t>El usuario ingresa los datos personales(nombre, rut, dirección, telefono, fecha de nacimiento) del  Hostel Worker.</t>
+  </si>
+  <si>
+    <t>Hostel Worker agregado correctamente al sistema</t>
+  </si>
+  <si>
+    <t>Hostel Worker no agregado anteriormente, el usuario debe ser Administrador.</t>
   </si>
 </sst>
 </file>
@@ -1094,7 +1100,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="61">
+  <cellXfs count="62">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1122,19 +1128,36 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1147,6 +1170,16 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1157,34 +1190,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="14" fontId="1" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1469,7 +1474,7 @@
   <dimension ref="B1:I34"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K31" sqref="K31"/>
+      <selection activeCell="C17" sqref="C17:E17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1486,237 +1491,247 @@
   <sheetData>
     <row r="1" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="42" t="s">
+      <c r="B2" s="57" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="29"/>
-      <c r="D2" s="43"/>
-      <c r="E2" s="44" t="s">
+      <c r="C2" s="33"/>
+      <c r="D2" s="58"/>
+      <c r="E2" s="59" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-      <c r="H2" s="46"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="61"/>
       <c r="I2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="37" t="s">
+      <c r="B3" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="38"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="47" t="s">
+      <c r="C3" s="47"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="51" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="47"/>
-      <c r="G3" s="47"/>
-      <c r="H3" s="47"/>
-      <c r="I3" s="48"/>
+      <c r="F3" s="51"/>
+      <c r="G3" s="51"/>
+      <c r="H3" s="51"/>
+      <c r="I3" s="52"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="38"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="47" t="s">
-        <v>35</v>
-      </c>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="47"/>
-      <c r="I4" s="48"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="51" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4" s="51"/>
+      <c r="G4" s="51"/>
+      <c r="H4" s="51"/>
+      <c r="I4" s="52"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="37" t="s">
+      <c r="B5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="38"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="50" t="s">
-        <v>36</v>
-      </c>
-      <c r="F5" s="40" t="s">
+      <c r="C5" s="47"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="F5" s="49" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="40"/>
-      <c r="H5" s="40"/>
-      <c r="I5" s="41"/>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="50"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="38"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="47" t="s">
-        <v>26</v>
-      </c>
-      <c r="F6" s="47"/>
-      <c r="G6" s="47"/>
-      <c r="H6" s="47"/>
-      <c r="I6" s="48"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="51" t="s">
+        <v>46</v>
+      </c>
+      <c r="F6" s="51"/>
+      <c r="G6" s="51"/>
+      <c r="H6" s="51"/>
+      <c r="I6" s="52"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="37" t="s">
+      <c r="B7" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="38"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="47" t="s">
-        <v>27</v>
-      </c>
-      <c r="F7" s="47"/>
-      <c r="G7" s="47"/>
-      <c r="H7" s="47"/>
-      <c r="I7" s="48"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="51" t="s">
+        <v>45</v>
+      </c>
+      <c r="F7" s="51"/>
+      <c r="G7" s="51"/>
+      <c r="H7" s="51"/>
+      <c r="I7" s="52"/>
     </row>
     <row r="8" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="53" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="33"/>
+      <c r="C8" s="54"/>
+      <c r="D8" s="55"/>
       <c r="E8" s="11" t="s">
         <v>25</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="49">
+      <c r="G8" s="21">
         <v>42111</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>9</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="24" t="s">
+      <c r="B10" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="25"/>
-      <c r="F10" s="25"/>
-      <c r="G10" s="25"/>
-      <c r="H10" s="25"/>
-      <c r="I10" s="26"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="42"/>
     </row>
     <row r="11" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="21" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="22"/>
-      <c r="D11" s="22"/>
-      <c r="E11" s="22"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="22"/>
-      <c r="H11" s="22"/>
-      <c r="I11" s="23"/>
+      <c r="B11" s="56" t="s">
+        <v>32</v>
+      </c>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="39"/>
     </row>
     <row r="12" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="24" t="s">
+      <c r="B13" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
-      <c r="E13" s="25"/>
-      <c r="F13" s="25"/>
-      <c r="G13" s="25"/>
-      <c r="H13" s="25"/>
-      <c r="I13" s="26"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="42"/>
     </row>
     <row r="14" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="21" t="s">
-        <v>33</v>
-      </c>
-      <c r="C14" s="22"/>
-      <c r="D14" s="22"/>
-      <c r="E14" s="22"/>
-      <c r="F14" s="22"/>
-      <c r="G14" s="22"/>
-      <c r="H14" s="22"/>
-      <c r="I14" s="23"/>
+      <c r="B14" s="56" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="39"/>
     </row>
     <row r="15" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="35"/>
-      <c r="D16" s="35"/>
-      <c r="E16" s="35"/>
-      <c r="F16" s="35"/>
-      <c r="G16" s="35"/>
-      <c r="H16" s="35"/>
-      <c r="I16" s="36"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="45"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="15">
         <v>1</v>
       </c>
-      <c r="C17" s="57" t="s">
-        <v>37</v>
-      </c>
-      <c r="D17" s="27"/>
-      <c r="E17" s="28"/>
+      <c r="C17" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="30"/>
+      <c r="E17" s="31"/>
       <c r="F17" s="15">
         <v>3</v>
       </c>
-      <c r="G17" s="27" t="s">
-        <v>39</v>
-      </c>
-      <c r="H17" s="29"/>
-      <c r="I17" s="30"/>
+      <c r="G17" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="H17" s="33"/>
+      <c r="I17" s="34"/>
     </row>
     <row r="18" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="16">
         <v>2</v>
       </c>
-      <c r="C18" s="58" t="s">
-        <v>38</v>
-      </c>
-      <c r="D18" s="59"/>
-      <c r="E18" s="60"/>
+      <c r="C18" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="36"/>
+      <c r="E18" s="37"/>
       <c r="F18" s="16">
         <v>4</v>
       </c>
-      <c r="G18" s="22" t="s">
+      <c r="G18" s="38" t="s">
+        <v>35</v>
+      </c>
+      <c r="H18" s="38"/>
+      <c r="I18" s="39"/>
+    </row>
+    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B19" s="18">
+        <v>5</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F19" s="18">
+        <v>6</v>
+      </c>
+      <c r="G19" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="H18" s="22"/>
-      <c r="I18" s="23"/>
-    </row>
-    <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="18"/>
-      <c r="F19" s="18"/>
     </row>
     <row r="20" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="24" t="s">
+      <c r="B21" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="25"/>
-      <c r="D21" s="25"/>
-      <c r="E21" s="25"/>
-      <c r="F21" s="25"/>
-      <c r="G21" s="25"/>
-      <c r="H21" s="25"/>
-      <c r="I21" s="26"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
+      <c r="G21" s="41"/>
+      <c r="H21" s="41"/>
+      <c r="I21" s="42"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="20" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
@@ -1730,7 +1745,7 @@
         <v>43</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
@@ -1741,16 +1756,16 @@
     </row>
     <row r="27" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="52" t="s">
+      <c r="B28" s="24" t="s">
         <v>14</v>
       </c>
-      <c r="C28" s="53"/>
-      <c r="D28" s="53"/>
-      <c r="E28" s="53"/>
-      <c r="F28" s="53"/>
-      <c r="G28" s="53"/>
-      <c r="H28" s="53"/>
-      <c r="I28" s="54"/>
+      <c r="C28" s="25"/>
+      <c r="D28" s="25"/>
+      <c r="E28" s="25"/>
+      <c r="F28" s="25"/>
+      <c r="G28" s="25"/>
+      <c r="H28" s="25"/>
+      <c r="I28" s="26"/>
     </row>
     <row r="29" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B29" s="3" t="s">
@@ -1759,16 +1774,16 @@
       <c r="C29" s="4"/>
       <c r="D29" s="5"/>
       <c r="E29" s="7" t="s">
-        <v>32</v>
-      </c>
-      <c r="F29" s="55" t="s">
+        <v>30</v>
+      </c>
+      <c r="F29" s="27" t="s">
         <v>16</v>
       </c>
       <c r="G29" s="5"/>
-      <c r="H29" s="55" t="s">
-        <v>36</v>
-      </c>
-      <c r="I29" s="56"/>
+      <c r="H29" s="27" t="s">
+        <v>34</v>
+      </c>
+      <c r="I29" s="28"/>
     </row>
     <row r="30" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B30" s="3" t="s">
@@ -1777,16 +1792,16 @@
       <c r="C30" s="4"/>
       <c r="D30" s="5"/>
       <c r="E30" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="F30" s="55" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" s="27" t="s">
         <v>18</v>
       </c>
       <c r="G30" s="5"/>
-      <c r="H30" s="55" t="s">
-        <v>29</v>
-      </c>
-      <c r="I30" s="56"/>
+      <c r="H30" s="27" t="s">
+        <v>27</v>
+      </c>
+      <c r="I30" s="28"/>
     </row>
     <row r="31" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B31" s="8" t="s">
@@ -1795,29 +1810,29 @@
       <c r="C31" s="9"/>
       <c r="D31" s="10"/>
       <c r="E31" s="13" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F31" s="17" t="s">
         <v>20</v>
       </c>
       <c r="G31" s="10"/>
       <c r="H31" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="I31" s="51"/>
+        <v>27</v>
+      </c>
+      <c r="I31" s="23"/>
     </row>
     <row r="32" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="52" t="s">
+      <c r="B33" s="24" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="53"/>
-      <c r="D33" s="53"/>
-      <c r="E33" s="53"/>
-      <c r="F33" s="53"/>
-      <c r="G33" s="53"/>
-      <c r="H33" s="53"/>
-      <c r="I33" s="54"/>
+      <c r="C33" s="25"/>
+      <c r="D33" s="25"/>
+      <c r="E33" s="25"/>
+      <c r="F33" s="25"/>
+      <c r="G33" s="25"/>
+      <c r="H33" s="25"/>
+      <c r="I33" s="26"/>
     </row>
     <row r="34" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B34" s="8"/>
@@ -1827,7 +1842,7 @@
       <c r="F34" s="9"/>
       <c r="G34" s="9"/>
       <c r="H34" s="9"/>
-      <c r="I34" s="51"/>
+      <c r="I34" s="23"/>
     </row>
   </sheetData>
   <mergeCells count="23">

</xml_diff>

<commit_message>
[Update] CDUN Agregar Hostel Worker
</commit_message>
<xml_diff>
--- a/análisis/Casos de Uso Narrativos/CDUN - (Administrar Personal) Agregar Hostel Worker.xlsx
+++ b/análisis/Casos de Uso Narrativos/CDUN - (Administrar Personal) Agregar Hostel Worker.xlsx
@@ -624,18 +624,12 @@
     <t>????</t>
   </si>
   <si>
-    <t>El usuario ingresa los un nombre de usuario y contraseña para el HostelWorker</t>
-  </si>
-  <si>
     <t>El rut del Hostel Worker ya ha sido ingresado. Se indica el error y se pide ingresar un nuevo rut.</t>
   </si>
   <si>
     <t>El nombre de usuario del Hostel Worker ya se encuentra usado. Se indica el error y se pide ingresar un nuevo nombre de usuario.</t>
   </si>
   <si>
-    <t>El caso de uso comienza cuando el administrador seleciona agregar Hostel Worker</t>
-  </si>
-  <si>
     <t>El sistema valida los datos y los ingresa al sistema.</t>
   </si>
   <si>
@@ -651,13 +645,19 @@
     <t>5b</t>
   </si>
   <si>
-    <t>El usuario ingresa los datos personales(nombre, rut, dirección, telefono, fecha de nacimiento) del  Hostel Worker.</t>
-  </si>
-  <si>
     <t>Hostel Worker agregado correctamente al sistema</t>
   </si>
   <si>
     <t>Hostel Worker no agregado anteriormente, el usuario debe ser Administrador.</t>
+  </si>
+  <si>
+    <t>Actor Admin: Seleciona agregar Hostel Worker</t>
+  </si>
+  <si>
+    <t>Actor Admin: Ingresa los datos personales(nombre, rut, dirección, telefono, fecha de nacimiento) del  Hostel Worker.</t>
+  </si>
+  <si>
+    <t>Actor Admin: ingresa los un nombre de usuario y contraseña para el HostelWorker</t>
   </si>
 </sst>
 </file>
@@ -1138,11 +1138,49 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -1152,44 +1190,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1473,8 +1473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I34"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17:E17"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1491,99 +1491,99 @@
   <sheetData>
     <row r="1" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="57" t="s">
+      <c r="B2" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="58"/>
-      <c r="E2" s="59" t="s">
+      <c r="C2" s="30"/>
+      <c r="D2" s="31"/>
+      <c r="E2" s="32" t="s">
         <v>24</v>
       </c>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="61"/>
+      <c r="F2" s="33"/>
+      <c r="G2" s="33"/>
+      <c r="H2" s="34"/>
       <c r="I2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="35" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="51" t="s">
+      <c r="C3" s="36"/>
+      <c r="D3" s="37"/>
+      <c r="E3" s="38" t="s">
         <v>23</v>
       </c>
-      <c r="F3" s="51"/>
-      <c r="G3" s="51"/>
-      <c r="H3" s="51"/>
-      <c r="I3" s="52"/>
+      <c r="F3" s="38"/>
+      <c r="G3" s="38"/>
+      <c r="H3" s="38"/>
+      <c r="I3" s="39"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="51" t="s">
+      <c r="C4" s="36"/>
+      <c r="D4" s="37"/>
+      <c r="E4" s="38" t="s">
         <v>33</v>
       </c>
-      <c r="F4" s="51"/>
-      <c r="G4" s="51"/>
-      <c r="H4" s="51"/>
-      <c r="I4" s="52"/>
+      <c r="F4" s="38"/>
+      <c r="G4" s="38"/>
+      <c r="H4" s="38"/>
+      <c r="I4" s="39"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="35" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="48"/>
+      <c r="C5" s="36"/>
+      <c r="D5" s="37"/>
       <c r="E5" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="F5" s="49" t="s">
+      <c r="F5" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="50"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="44"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="35" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="51" t="s">
-        <v>46</v>
-      </c>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="51"/>
-      <c r="I6" s="52"/>
+      <c r="C6" s="36"/>
+      <c r="D6" s="37"/>
+      <c r="E6" s="38" t="s">
+        <v>43</v>
+      </c>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="39"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="35" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="51" t="s">
-        <v>45</v>
-      </c>
-      <c r="F7" s="51"/>
-      <c r="G7" s="51"/>
-      <c r="H7" s="51"/>
-      <c r="I7" s="52"/>
+      <c r="C7" s="36"/>
+      <c r="D7" s="37"/>
+      <c r="E7" s="38" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="39"/>
     </row>
     <row r="8" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="53" t="s">
+      <c r="B8" s="45" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="54"/>
-      <c r="D8" s="55"/>
+      <c r="C8" s="46"/>
+      <c r="D8" s="47"/>
       <c r="E8" s="11" t="s">
         <v>25</v>
       </c>
@@ -1602,136 +1602,139 @@
     </row>
     <row r="9" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="42"/>
+      <c r="C10" s="49"/>
+      <c r="D10" s="49"/>
+      <c r="E10" s="49"/>
+      <c r="F10" s="49"/>
+      <c r="G10" s="49"/>
+      <c r="H10" s="49"/>
+      <c r="I10" s="50"/>
     </row>
     <row r="11" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="56" t="s">
+      <c r="B11" s="51" t="s">
         <v>32</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="39"/>
+      <c r="C11" s="52"/>
+      <c r="D11" s="52"/>
+      <c r="E11" s="52"/>
+      <c r="F11" s="52"/>
+      <c r="G11" s="52"/>
+      <c r="H11" s="52"/>
+      <c r="I11" s="53"/>
     </row>
     <row r="12" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="48" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="42"/>
+      <c r="C13" s="49"/>
+      <c r="D13" s="49"/>
+      <c r="E13" s="49"/>
+      <c r="F13" s="49"/>
+      <c r="G13" s="49"/>
+      <c r="H13" s="49"/>
+      <c r="I13" s="50"/>
     </row>
     <row r="14" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="56" t="s">
+      <c r="B14" s="51" t="s">
         <v>31</v>
       </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="39"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="53"/>
     </row>
     <row r="15" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="40" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="45"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
+      <c r="G16" s="41"/>
+      <c r="H16" s="41"/>
+      <c r="I16" s="42"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="15">
         <v>1</v>
       </c>
-      <c r="C17" s="29" t="s">
-        <v>38</v>
-      </c>
-      <c r="D17" s="30"/>
-      <c r="E17" s="31"/>
+      <c r="C17" s="54" t="s">
+        <v>44</v>
+      </c>
+      <c r="D17" s="55"/>
+      <c r="E17" s="56"/>
       <c r="F17" s="15">
-        <v>3</v>
-      </c>
-      <c r="G17" s="32" t="s">
-        <v>44</v>
-      </c>
-      <c r="H17" s="33"/>
-      <c r="I17" s="34"/>
+        <v>2</v>
+      </c>
+      <c r="G17" s="57" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" s="30"/>
+      <c r="I17" s="58"/>
     </row>
     <row r="18" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="16">
-        <v>2</v>
-      </c>
-      <c r="C18" s="35" t="s">
-        <v>41</v>
-      </c>
-      <c r="D18" s="36"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="16">
-        <v>4</v>
-      </c>
-      <c r="G18" s="38" t="s">
-        <v>35</v>
-      </c>
-      <c r="H18" s="38"/>
-      <c r="I18" s="39"/>
+        <v>3</v>
+      </c>
+      <c r="C18" s="59" t="s">
+        <v>45</v>
+      </c>
+      <c r="D18" s="60"/>
+      <c r="E18" s="61"/>
+      <c r="F18" s="16"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="53"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B19" s="18">
+        <v>4</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F19" s="18">
         <v>5</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="F19" s="18">
+      <c r="G19" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="20" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B20" s="18">
         <v>6</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="20" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="C20" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
     <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="40" t="s">
+      <c r="B21" s="48" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
-      <c r="G21" s="41"/>
-      <c r="H21" s="41"/>
-      <c r="I21" s="42"/>
+      <c r="C21" s="49"/>
+      <c r="D21" s="49"/>
+      <c r="E21" s="49"/>
+      <c r="F21" s="49"/>
+      <c r="G21" s="49"/>
+      <c r="H21" s="49"/>
+      <c r="I21" s="50"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B22" s="20" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D22" s="7"/>
       <c r="E22" s="7"/>
@@ -1742,10 +1745,10 @@
     </row>
     <row r="23" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B23" s="19" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="C23" s="13" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="D23" s="13"/>
       <c r="E23" s="13"/>
@@ -1846,12 +1849,11 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:I3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="G18:I18"/>
+    <mergeCell ref="B21:I21"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="F5:I5"/>
@@ -1864,11 +1866,12 @@
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="B13:I13"/>
     <mergeCell ref="B14:I14"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="B21:I21"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:I4"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[UPDATE] CDUN Adm. Personal + [ADD] RF07
</commit_message>
<xml_diff>
--- a/análisis/Casos de Uso Narrativos/CDUN - (Administrar Personal) Agregar Hostel Worker.xlsx
+++ b/análisis/Casos de Uso Narrativos/CDUN - (Administrar Personal) Agregar Hostel Worker.xlsx
@@ -271,7 +271,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G18" authorId="0" shapeId="0">
+    <comment ref="G20" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -295,7 +295,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="B22" authorId="0" shapeId="0">
+    <comment ref="B23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -319,7 +319,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C22" authorId="0" shapeId="0">
+    <comment ref="C23" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -340,6 +340,102 @@
           </rPr>
           <t xml:space="preserve">
 Descripción de la secuencia alternativa a la acción 1 (según ejemplo) del curso normal</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B27" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Andrés Vega Yáñez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Numero de veces que se realizará el CU en alguna unidad de tiempo.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F27" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Andrés Vega Yáñez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Rendimiento esperado de la secuencia de acciones del CU</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="B28" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Andrés Vega Yáñez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Vital, Alta, Moderada, Baja</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F28" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Andrés Vega Yáñez:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Urgencia en la realización de este CU. Alta, Moderada, Baja </t>
         </r>
       </text>
     </comment>
@@ -363,7 +459,7 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Numero de veces que se realizará el CU en alguna unidad de tiempo.</t>
+Estado actual en el desarrollo</t>
         </r>
       </text>
     </comment>
@@ -387,108 +483,12 @@
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-Rendimiento esperado de la secuencia de acciones del CU</t>
+Estabilidad de los requerimientos asociados a este CU.
+Alta, Moderada, Baja</t>
         </r>
       </text>
     </comment>
-    <comment ref="B30" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Andrés Vega Yáñez:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Vital, Alta, Moderada, Baja</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F30" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Andrés Vega Yáñez:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Urgencia en la realización de este CU. Alta, Moderada, Baja </t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B31" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Andrés Vega Yáñez:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Estado actual en el desarrollo</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="F31" authorId="0" shapeId="0">
-      <text>
-        <r>
-          <rPr>
-            <b/>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t>Andrés Vega Yáñez:</t>
-        </r>
-        <r>
-          <rPr>
-            <sz val="9"/>
-            <color indexed="81"/>
-            <rFont val="Tahoma"/>
-            <family val="2"/>
-          </rPr>
-          <t xml:space="preserve">
-Estabilidad de los requerimientos asociados a este CU.
-Alta, Moderada, Baja</t>
-        </r>
-      </text>
-    </comment>
-    <comment ref="B34" authorId="0" shapeId="0">
+    <comment ref="B32" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -517,7 +517,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="48" uniqueCount="45">
   <si>
     <t>Caso de uso</t>
   </si>
@@ -585,9 +585,6 @@
     <t>Comentarios</t>
   </si>
   <si>
-    <t>Administrar Personal</t>
-  </si>
-  <si>
     <t>Admin.</t>
   </si>
   <si>
@@ -597,9 +594,6 @@
     <t>Roberto Cordero</t>
   </si>
   <si>
-    <t>1.0</t>
-  </si>
-  <si>
     <t>Alta</t>
   </si>
   <si>
@@ -609,9 +603,6 @@
     <t>Vital</t>
   </si>
   <si>
-    <t>La mayor cantidad de veces que sea necesario</t>
-  </si>
-  <si>
     <t>Agrega los datos de un nuevo Hotel Worker para poder agregar un perfil de él al sistema.</t>
   </si>
   <si>
@@ -621,9 +612,6 @@
     <t>Primario| Esencial</t>
   </si>
   <si>
-    <t>????</t>
-  </si>
-  <si>
     <t>El rut del Hostel Worker ya ha sido ingresado. Se indica el error y se pide ingresar un nuevo rut.</t>
   </si>
   <si>
@@ -633,9 +621,6 @@
     <t>El sistema valida los datos y los ingresa al sistema.</t>
   </si>
   <si>
-    <t>Fin del caso de uso</t>
-  </si>
-  <si>
     <t>El sistema muestra un formulario para ingresar los datos.</t>
   </si>
   <si>
@@ -648,9 +633,6 @@
     <t>Hostel Worker agregado correctamente al sistema</t>
   </si>
   <si>
-    <t>Hostel Worker no agregado anteriormente, el usuario debe ser Administrador.</t>
-  </si>
-  <si>
     <t>Actor Admin: Seleciona agregar Hostel Worker</t>
   </si>
   <si>
@@ -658,6 +640,18 @@
   </si>
   <si>
     <t>Actor Admin: ingresa los un nombre de usuario y contraseña para el HostelWorker</t>
+  </si>
+  <si>
+    <t>Fin del caso de uso.</t>
+  </si>
+  <si>
+    <t>Hostel Worker no agregado anteriormente, el actor Admin debe seleccionar anteriormente el CU_Listar_Hostel_Workers</t>
+  </si>
+  <si>
+    <t>CU_Listar_Hostel_Workers</t>
+  </si>
+  <si>
+    <t>1.1</t>
   </si>
 </sst>
 </file>
@@ -725,7 +719,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="28">
+  <borders count="29">
     <border>
       <left/>
       <right/>
@@ -1096,11 +1090,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="62">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1115,7 +1120,6 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1138,30 +1142,33 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1171,25 +1178,41 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1471,10 +1494,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:I34"/>
+  <dimension ref="B1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="J26" sqref="J26"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="J29" sqref="J29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1491,369 +1514,383 @@
   <sheetData>
     <row r="1" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="29" t="s">
+      <c r="B2" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="30"/>
-      <c r="D2" s="31"/>
-      <c r="E2" s="32" t="s">
-        <v>24</v>
-      </c>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="34"/>
+      <c r="C2" s="33"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="57" t="s">
+        <v>23</v>
+      </c>
+      <c r="F2" s="58"/>
+      <c r="G2" s="58"/>
+      <c r="H2" s="59"/>
       <c r="I2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="36"/>
-      <c r="D3" s="37"/>
-      <c r="E3" s="38" t="s">
-        <v>23</v>
-      </c>
-      <c r="F3" s="38"/>
-      <c r="G3" s="38"/>
-      <c r="H3" s="38"/>
-      <c r="I3" s="39"/>
+      <c r="C3" s="47"/>
+      <c r="D3" s="48"/>
+      <c r="E3" s="49" t="s">
+        <v>22</v>
+      </c>
+      <c r="F3" s="49"/>
+      <c r="G3" s="49"/>
+      <c r="H3" s="49"/>
+      <c r="I3" s="50"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="46" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="37"/>
-      <c r="E4" s="38" t="s">
-        <v>33</v>
-      </c>
-      <c r="F4" s="38"/>
-      <c r="G4" s="38"/>
-      <c r="H4" s="38"/>
-      <c r="I4" s="39"/>
+      <c r="C4" s="47"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="49" t="s">
+        <v>30</v>
+      </c>
+      <c r="F4" s="49"/>
+      <c r="G4" s="49"/>
+      <c r="H4" s="49"/>
+      <c r="I4" s="50"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="46" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="36"/>
-      <c r="D5" s="37"/>
-      <c r="E5" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="F5" s="43" t="s">
-        <v>22</v>
-      </c>
-      <c r="G5" s="43"/>
-      <c r="H5" s="43"/>
-      <c r="I5" s="44"/>
+      <c r="C5" s="47"/>
+      <c r="D5" s="48"/>
+      <c r="E5" s="21"/>
+      <c r="F5" s="49" t="s">
+        <v>43</v>
+      </c>
+      <c r="G5" s="49"/>
+      <c r="H5" s="49"/>
+      <c r="I5" s="50"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="46" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="36"/>
-      <c r="D6" s="37"/>
-      <c r="E6" s="38" t="s">
-        <v>43</v>
-      </c>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="38"/>
-      <c r="I6" s="39"/>
+      <c r="C6" s="47"/>
+      <c r="D6" s="48"/>
+      <c r="E6" s="49" t="s">
+        <v>42</v>
+      </c>
+      <c r="F6" s="49"/>
+      <c r="G6" s="49"/>
+      <c r="H6" s="49"/>
+      <c r="I6" s="50"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="46" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="36"/>
-      <c r="D7" s="37"/>
-      <c r="E7" s="38" t="s">
-        <v>42</v>
-      </c>
-      <c r="F7" s="38"/>
-      <c r="G7" s="38"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="39"/>
+      <c r="C7" s="47"/>
+      <c r="D7" s="48"/>
+      <c r="E7" s="49" t="s">
+        <v>37</v>
+      </c>
+      <c r="F7" s="49"/>
+      <c r="G7" s="49"/>
+      <c r="H7" s="49"/>
+      <c r="I7" s="50"/>
     </row>
     <row r="8" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="45" t="s">
+      <c r="B8" s="51" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="46"/>
-      <c r="D8" s="47"/>
+      <c r="C8" s="52"/>
+      <c r="D8" s="53"/>
       <c r="E8" s="11" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F8" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="21">
+      <c r="G8" s="20">
         <v>42111</v>
       </c>
       <c r="H8" s="11" t="s">
         <v>9</v>
       </c>
       <c r="I8" s="12" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
     </row>
     <row r="9" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="48" t="s">
+      <c r="B10" s="40" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="49"/>
-      <c r="D10" s="49"/>
-      <c r="E10" s="49"/>
-      <c r="F10" s="49"/>
-      <c r="G10" s="49"/>
-      <c r="H10" s="49"/>
-      <c r="I10" s="50"/>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
+      <c r="G10" s="41"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="42"/>
     </row>
     <row r="11" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="51" t="s">
-        <v>32</v>
-      </c>
-      <c r="C11" s="52"/>
-      <c r="D11" s="52"/>
-      <c r="E11" s="52"/>
-      <c r="F11" s="52"/>
-      <c r="G11" s="52"/>
-      <c r="H11" s="52"/>
-      <c r="I11" s="53"/>
+      <c r="B11" s="54" t="s">
+        <v>29</v>
+      </c>
+      <c r="C11" s="38"/>
+      <c r="D11" s="38"/>
+      <c r="E11" s="38"/>
+      <c r="F11" s="38"/>
+      <c r="G11" s="38"/>
+      <c r="H11" s="38"/>
+      <c r="I11" s="39"/>
     </row>
     <row r="12" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="40" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="49"/>
-      <c r="D13" s="49"/>
-      <c r="E13" s="49"/>
-      <c r="F13" s="49"/>
-      <c r="G13" s="49"/>
-      <c r="H13" s="49"/>
-      <c r="I13" s="50"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
+      <c r="G13" s="41"/>
+      <c r="H13" s="41"/>
+      <c r="I13" s="42"/>
     </row>
     <row r="14" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B14" s="51" t="s">
-        <v>31</v>
-      </c>
-      <c r="C14" s="52"/>
-      <c r="D14" s="52"/>
-      <c r="E14" s="52"/>
-      <c r="F14" s="52"/>
-      <c r="G14" s="52"/>
-      <c r="H14" s="52"/>
-      <c r="I14" s="53"/>
+      <c r="B14" s="54" t="s">
+        <v>28</v>
+      </c>
+      <c r="C14" s="38"/>
+      <c r="D14" s="38"/>
+      <c r="E14" s="38"/>
+      <c r="F14" s="38"/>
+      <c r="G14" s="38"/>
+      <c r="H14" s="38"/>
+      <c r="I14" s="39"/>
     </row>
     <row r="15" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="40" t="s">
+      <c r="B16" s="43" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
-      <c r="G16" s="41"/>
-      <c r="H16" s="41"/>
-      <c r="I16" s="42"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="44"/>
+      <c r="E16" s="44"/>
+      <c r="F16" s="44"/>
+      <c r="G16" s="44"/>
+      <c r="H16" s="44"/>
+      <c r="I16" s="45"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B17" s="15">
+      <c r="B17" s="14">
         <v>1</v>
       </c>
-      <c r="C17" s="54" t="s">
-        <v>44</v>
-      </c>
-      <c r="D17" s="55"/>
-      <c r="E17" s="56"/>
-      <c r="F17" s="15">
+      <c r="C17" s="29" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="30"/>
+      <c r="E17" s="31"/>
+      <c r="F17" s="14">
         <v>2</v>
       </c>
-      <c r="G17" s="57" t="s">
+      <c r="G17" s="32" t="s">
+        <v>34</v>
+      </c>
+      <c r="H17" s="33"/>
+      <c r="I17" s="34"/>
+    </row>
+    <row r="18" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B18" s="64">
+        <v>3</v>
+      </c>
+      <c r="C18" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="H17" s="30"/>
-      <c r="I17" s="58"/>
-    </row>
-    <row r="18" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B18" s="16">
-        <v>3</v>
-      </c>
-      <c r="C18" s="59" t="s">
-        <v>45</v>
-      </c>
-      <c r="D18" s="60"/>
-      <c r="E18" s="61"/>
-      <c r="F18" s="16"/>
-      <c r="G18" s="52"/>
-      <c r="H18" s="52"/>
-      <c r="I18" s="53"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="63"/>
+      <c r="F18" s="64"/>
+      <c r="G18" s="26"/>
+      <c r="H18" s="28"/>
+      <c r="I18" s="27"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="18">
+      <c r="B19" s="60">
         <v>4</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F19" s="18">
+      <c r="C19" s="61" t="s">
+        <v>40</v>
+      </c>
+      <c r="D19" s="62"/>
+      <c r="E19" s="63"/>
+      <c r="F19" s="60">
         <v>5</v>
       </c>
-      <c r="G19" s="1" t="s">
-        <v>37</v>
-      </c>
+      <c r="G19" s="61" t="s">
+        <v>33</v>
+      </c>
+      <c r="H19" s="62"/>
+      <c r="I19" s="63"/>
     </row>
     <row r="20" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B20" s="18">
+      <c r="B20" s="15">
         <v>6</v>
       </c>
-      <c r="C20" s="1" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="21" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B21" s="48" t="s">
+      <c r="C20" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D20" s="36"/>
+      <c r="E20" s="37"/>
+      <c r="F20" s="15"/>
+      <c r="G20" s="38"/>
+      <c r="H20" s="38"/>
+      <c r="I20" s="39"/>
+    </row>
+    <row r="21" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B21" s="17"/>
+      <c r="F21" s="17"/>
+    </row>
+    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B22" s="40" t="s">
         <v>13</v>
       </c>
-      <c r="C21" s="49"/>
-      <c r="D21" s="49"/>
-      <c r="E21" s="49"/>
-      <c r="F21" s="49"/>
-      <c r="G21" s="49"/>
-      <c r="H21" s="49"/>
-      <c r="I21" s="50"/>
-    </row>
-    <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="20" t="s">
-        <v>40</v>
-      </c>
-      <c r="C22" s="7" t="s">
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
+      <c r="G22" s="41"/>
+      <c r="H22" s="41"/>
+      <c r="I22" s="42"/>
+    </row>
+    <row r="23" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B23" s="19" t="s">
         <v>35</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="7"/>
-      <c r="F22" s="7"/>
-      <c r="G22" s="7"/>
-      <c r="H22" s="7"/>
-      <c r="I22" s="6"/>
-    </row>
-    <row r="23" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B23" s="19" t="s">
-        <v>41</v>
-      </c>
-      <c r="C23" s="13" t="s">
+      <c r="C23" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D23" s="7"/>
+      <c r="E23" s="7"/>
+      <c r="F23" s="7"/>
+      <c r="G23" s="7"/>
+      <c r="H23" s="7"/>
+      <c r="I23" s="6"/>
+    </row>
+    <row r="24" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B24" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="D23" s="13"/>
-      <c r="E23" s="13"/>
-      <c r="F23" s="13"/>
-      <c r="G23" s="13"/>
-      <c r="H23" s="13"/>
-      <c r="I23" s="14"/>
-    </row>
-    <row r="27" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+      <c r="C24" s="65" t="s">
+        <v>32</v>
+      </c>
+      <c r="D24" s="66"/>
+      <c r="E24" s="66"/>
+      <c r="F24" s="66"/>
+      <c r="G24" s="66"/>
+      <c r="H24" s="66"/>
+      <c r="I24" s="67"/>
+    </row>
+    <row r="25" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="26" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B26" s="23" t="s">
+        <v>14</v>
+      </c>
+      <c r="C26" s="24"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="24"/>
+      <c r="G26" s="24"/>
+      <c r="H26" s="24"/>
+      <c r="I26" s="25"/>
+    </row>
+    <row r="27" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C27" s="4"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F27" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="G27" s="5"/>
+      <c r="H27" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="I27" s="27"/>
+    </row>
     <row r="28" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B28" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="C28" s="25"/>
-      <c r="D28" s="25"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="25"/>
-      <c r="G28" s="25"/>
-      <c r="H28" s="25"/>
-      <c r="I28" s="26"/>
-    </row>
-    <row r="29" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B29" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="C29" s="4"/>
-      <c r="D29" s="5"/>
-      <c r="E29" s="7" t="s">
-        <v>30</v>
-      </c>
-      <c r="F29" s="27" t="s">
-        <v>16</v>
-      </c>
-      <c r="G29" s="5"/>
-      <c r="H29" s="27" t="s">
-        <v>34</v>
-      </c>
-      <c r="I29" s="28"/>
-    </row>
-    <row r="30" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B30" s="3" t="s">
+      <c r="B28" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="C30" s="4"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="F30" s="27" t="s">
+      <c r="C28" s="4"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="F28" s="26" t="s">
         <v>18</v>
       </c>
-      <c r="G30" s="5"/>
-      <c r="H30" s="27" t="s">
-        <v>27</v>
-      </c>
-      <c r="I30" s="28"/>
-    </row>
-    <row r="31" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B31" s="8" t="s">
+      <c r="G28" s="5"/>
+      <c r="H28" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="I28" s="27"/>
+    </row>
+    <row r="29" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B29" s="8" t="s">
         <v>19</v>
       </c>
-      <c r="C31" s="9"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="F31" s="17" t="s">
+      <c r="C29" s="9"/>
+      <c r="D29" s="10"/>
+      <c r="E29" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="F29" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="G31" s="10"/>
-      <c r="H31" s="17" t="s">
-        <v>27</v>
-      </c>
-      <c r="I31" s="23"/>
-    </row>
-    <row r="32" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="33" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B33" s="24" t="s">
+      <c r="G29" s="10"/>
+      <c r="H29" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="I29" s="22"/>
+    </row>
+    <row r="30" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="31" spans="2:9" x14ac:dyDescent="0.25">
+      <c r="B31" s="23" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="25"/>
-      <c r="D33" s="25"/>
-      <c r="E33" s="25"/>
-      <c r="F33" s="25"/>
-      <c r="G33" s="25"/>
-      <c r="H33" s="25"/>
-      <c r="I33" s="26"/>
-    </row>
-    <row r="34" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B34" s="8"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="9"/>
-      <c r="E34" s="9"/>
-      <c r="F34" s="9"/>
-      <c r="G34" s="9"/>
-      <c r="H34" s="9"/>
-      <c r="I34" s="23"/>
+      <c r="C31" s="24"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="24"/>
+      <c r="H31" s="24"/>
+      <c r="I31" s="25"/>
+    </row>
+    <row r="32" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B32" s="8"/>
+      <c r="C32" s="9"/>
+      <c r="D32" s="9"/>
+      <c r="E32" s="9"/>
+      <c r="F32" s="9"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="23">
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="G18:I18"/>
-    <mergeCell ref="B21:I21"/>
+  <mergeCells count="27">
+    <mergeCell ref="C24:I24"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="E2:H2"/>
+    <mergeCell ref="B3:D3"/>
+    <mergeCell ref="E3:I3"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E4:I4"/>
     <mergeCell ref="B16:I16"/>
     <mergeCell ref="B5:D5"/>
     <mergeCell ref="F5:I5"/>
@@ -1866,12 +1903,14 @@
     <mergeCell ref="B11:I11"/>
     <mergeCell ref="B13:I13"/>
     <mergeCell ref="B14:I14"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="E2:H2"/>
-    <mergeCell ref="B3:D3"/>
-    <mergeCell ref="E3:I3"/>
-    <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E4:I4"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="G17:I17"/>
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="G19:I19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
[Added] CDUN- Administrar Inventario
Además se modifican partes del texto de los CDUN de Administrar
personal.
</commit_message>
<xml_diff>
--- a/análisis/Casos de Uso Narrativos/CDUN - (Administrar Personal) Agregar Hostel Worker.xlsx
+++ b/análisis/Casos de Uso Narrativos/CDUN - (Administrar Personal) Agregar Hostel Worker.xlsx
@@ -1143,64 +1143,8 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="24" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1212,6 +1156,62 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1496,8 +1496,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:I32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="J29" sqref="J29"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19:I19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -1514,97 +1514,97 @@
   <sheetData>
     <row r="1" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B2" s="55" t="s">
+      <c r="B2" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="33"/>
-      <c r="D2" s="56"/>
-      <c r="E2" s="57" t="s">
+      <c r="C2" s="35"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="37" t="s">
         <v>23</v>
       </c>
-      <c r="F2" s="58"/>
-      <c r="G2" s="58"/>
-      <c r="H2" s="59"/>
+      <c r="F2" s="38"/>
+      <c r="G2" s="38"/>
+      <c r="H2" s="39"/>
       <c r="I2" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="3" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B3" s="46" t="s">
+      <c r="B3" s="40" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="47"/>
-      <c r="D3" s="48"/>
-      <c r="E3" s="49" t="s">
+      <c r="C3" s="41"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="43" t="s">
         <v>22</v>
       </c>
-      <c r="F3" s="49"/>
-      <c r="G3" s="49"/>
-      <c r="H3" s="49"/>
-      <c r="I3" s="50"/>
+      <c r="F3" s="43"/>
+      <c r="G3" s="43"/>
+      <c r="H3" s="43"/>
+      <c r="I3" s="44"/>
     </row>
     <row r="4" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B4" s="46" t="s">
+      <c r="B4" s="40" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="48"/>
-      <c r="E4" s="49" t="s">
+      <c r="C4" s="41"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="43" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="49"/>
-      <c r="G4" s="49"/>
-      <c r="H4" s="49"/>
-      <c r="I4" s="50"/>
+      <c r="F4" s="43"/>
+      <c r="G4" s="43"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="44"/>
     </row>
     <row r="5" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B5" s="46" t="s">
+      <c r="B5" s="40" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="47"/>
-      <c r="D5" s="48"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="42"/>
       <c r="E5" s="21"/>
-      <c r="F5" s="49" t="s">
+      <c r="F5" s="43" t="s">
         <v>43</v>
       </c>
-      <c r="G5" s="49"/>
-      <c r="H5" s="49"/>
-      <c r="I5" s="50"/>
+      <c r="G5" s="43"/>
+      <c r="H5" s="43"/>
+      <c r="I5" s="44"/>
     </row>
     <row r="6" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B6" s="46" t="s">
+      <c r="B6" s="40" t="s">
         <v>5</v>
       </c>
-      <c r="C6" s="47"/>
-      <c r="D6" s="48"/>
-      <c r="E6" s="49" t="s">
+      <c r="C6" s="41"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="43" t="s">
         <v>42</v>
       </c>
-      <c r="F6" s="49"/>
-      <c r="G6" s="49"/>
-      <c r="H6" s="49"/>
-      <c r="I6" s="50"/>
+      <c r="F6" s="43"/>
+      <c r="G6" s="43"/>
+      <c r="H6" s="43"/>
+      <c r="I6" s="44"/>
     </row>
     <row r="7" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B7" s="46" t="s">
+      <c r="B7" s="40" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="47"/>
-      <c r="D7" s="48"/>
-      <c r="E7" s="49" t="s">
+      <c r="C7" s="41"/>
+      <c r="D7" s="42"/>
+      <c r="E7" s="43" t="s">
         <v>37</v>
       </c>
-      <c r="F7" s="49"/>
-      <c r="G7" s="49"/>
-      <c r="H7" s="49"/>
-      <c r="I7" s="50"/>
+      <c r="F7" s="43"/>
+      <c r="G7" s="43"/>
+      <c r="H7" s="43"/>
+      <c r="I7" s="44"/>
     </row>
     <row r="8" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="48" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="52"/>
-      <c r="D8" s="53"/>
+      <c r="C8" s="49"/>
+      <c r="D8" s="50"/>
       <c r="E8" s="11" t="s">
         <v>24</v>
       </c>
@@ -1623,146 +1623,146 @@
     </row>
     <row r="9" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B10" s="40" t="s">
+      <c r="B10" s="51" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
-      <c r="G10" s="41"/>
-      <c r="H10" s="41"/>
-      <c r="I10" s="42"/>
+      <c r="C10" s="52"/>
+      <c r="D10" s="52"/>
+      <c r="E10" s="52"/>
+      <c r="F10" s="52"/>
+      <c r="G10" s="52"/>
+      <c r="H10" s="52"/>
+      <c r="I10" s="53"/>
     </row>
     <row r="11" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B11" s="54" t="s">
         <v>29</v>
       </c>
-      <c r="C11" s="38"/>
-      <c r="D11" s="38"/>
-      <c r="E11" s="38"/>
-      <c r="F11" s="38"/>
-      <c r="G11" s="38"/>
-      <c r="H11" s="38"/>
-      <c r="I11" s="39"/>
+      <c r="C11" s="55"/>
+      <c r="D11" s="55"/>
+      <c r="E11" s="55"/>
+      <c r="F11" s="55"/>
+      <c r="G11" s="55"/>
+      <c r="H11" s="55"/>
+      <c r="I11" s="56"/>
     </row>
     <row r="12" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="13" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B13" s="40" t="s">
+      <c r="B13" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
-      <c r="G13" s="41"/>
-      <c r="H13" s="41"/>
-      <c r="I13" s="42"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="53"/>
     </row>
     <row r="14" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B14" s="54" t="s">
         <v>28</v>
       </c>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="39"/>
+      <c r="C14" s="55"/>
+      <c r="D14" s="55"/>
+      <c r="E14" s="55"/>
+      <c r="F14" s="55"/>
+      <c r="G14" s="55"/>
+      <c r="H14" s="55"/>
+      <c r="I14" s="56"/>
     </row>
     <row r="15" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="16" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="45" t="s">
         <v>12</v>
       </c>
-      <c r="C16" s="44"/>
-      <c r="D16" s="44"/>
-      <c r="E16" s="44"/>
-      <c r="F16" s="44"/>
-      <c r="G16" s="44"/>
-      <c r="H16" s="44"/>
-      <c r="I16" s="45"/>
+      <c r="C16" s="46"/>
+      <c r="D16" s="46"/>
+      <c r="E16" s="46"/>
+      <c r="F16" s="46"/>
+      <c r="G16" s="46"/>
+      <c r="H16" s="46"/>
+      <c r="I16" s="47"/>
     </row>
     <row r="17" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B17" s="14">
         <v>1</v>
       </c>
-      <c r="C17" s="29" t="s">
+      <c r="C17" s="57" t="s">
         <v>38</v>
       </c>
-      <c r="D17" s="30"/>
-      <c r="E17" s="31"/>
+      <c r="D17" s="58"/>
+      <c r="E17" s="59"/>
       <c r="F17" s="14">
         <v>2</v>
       </c>
-      <c r="G17" s="32" t="s">
+      <c r="G17" s="60" t="s">
         <v>34</v>
       </c>
-      <c r="H17" s="33"/>
-      <c r="I17" s="34"/>
+      <c r="H17" s="35"/>
+      <c r="I17" s="61"/>
     </row>
     <row r="18" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B18" s="64">
+      <c r="B18" s="30">
         <v>3</v>
       </c>
-      <c r="C18" s="61" t="s">
+      <c r="C18" s="65" t="s">
         <v>39</v>
       </c>
-      <c r="D18" s="62"/>
-      <c r="E18" s="63"/>
-      <c r="F18" s="64"/>
+      <c r="D18" s="66"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="30"/>
       <c r="G18" s="26"/>
       <c r="H18" s="28"/>
       <c r="I18" s="27"/>
     </row>
     <row r="19" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B19" s="60">
+      <c r="B19" s="29">
         <v>4</v>
       </c>
-      <c r="C19" s="61" t="s">
+      <c r="C19" s="65" t="s">
         <v>40</v>
       </c>
-      <c r="D19" s="62"/>
-      <c r="E19" s="63"/>
-      <c r="F19" s="60">
+      <c r="D19" s="66"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="29">
         <v>5</v>
       </c>
-      <c r="G19" s="61" t="s">
+      <c r="G19" s="65" t="s">
         <v>33</v>
       </c>
-      <c r="H19" s="62"/>
-      <c r="I19" s="63"/>
+      <c r="H19" s="66"/>
+      <c r="I19" s="67"/>
     </row>
     <row r="20" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" s="15">
         <v>6</v>
       </c>
-      <c r="C20" s="35" t="s">
+      <c r="C20" s="62" t="s">
         <v>41</v>
       </c>
-      <c r="D20" s="36"/>
-      <c r="E20" s="37"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="64"/>
       <c r="F20" s="15"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="39"/>
+      <c r="G20" s="55"/>
+      <c r="H20" s="55"/>
+      <c r="I20" s="56"/>
     </row>
     <row r="21" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="17"/>
       <c r="F21" s="17"/>
     </row>
     <row r="22" spans="2:9" x14ac:dyDescent="0.25">
-      <c r="B22" s="40" t="s">
+      <c r="B22" s="51" t="s">
         <v>13</v>
       </c>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
-      <c r="G22" s="41"/>
-      <c r="H22" s="41"/>
-      <c r="I22" s="42"/>
+      <c r="C22" s="52"/>
+      <c r="D22" s="52"/>
+      <c r="E22" s="52"/>
+      <c r="F22" s="52"/>
+      <c r="G22" s="52"/>
+      <c r="H22" s="52"/>
+      <c r="I22" s="53"/>
     </row>
     <row r="23" spans="2:9" x14ac:dyDescent="0.25">
       <c r="B23" s="19" t="s">
@@ -1782,15 +1782,15 @@
       <c r="B24" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="C24" s="65" t="s">
+      <c r="C24" s="31" t="s">
         <v>32</v>
       </c>
-      <c r="D24" s="66"/>
-      <c r="E24" s="66"/>
-      <c r="F24" s="66"/>
-      <c r="G24" s="66"/>
-      <c r="H24" s="66"/>
-      <c r="I24" s="67"/>
+      <c r="D24" s="32"/>
+      <c r="E24" s="32"/>
+      <c r="F24" s="32"/>
+      <c r="G24" s="32"/>
+      <c r="H24" s="32"/>
+      <c r="I24" s="33"/>
     </row>
     <row r="25" spans="2:9" ht="16.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="2:9" x14ac:dyDescent="0.25">
@@ -1884,6 +1884,17 @@
     </row>
   </sheetData>
   <mergeCells count="27">
+    <mergeCell ref="C20:E20"/>
+    <mergeCell ref="G20:I20"/>
+    <mergeCell ref="B22:I22"/>
+    <mergeCell ref="C18:E18"/>
+    <mergeCell ref="C19:E19"/>
+    <mergeCell ref="G19:I19"/>
+    <mergeCell ref="B11:I11"/>
+    <mergeCell ref="B13:I13"/>
+    <mergeCell ref="B14:I14"/>
+    <mergeCell ref="C17:E17"/>
+    <mergeCell ref="G17:I17"/>
     <mergeCell ref="C24:I24"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="E2:H2"/>
@@ -1900,17 +1911,6 @@
     <mergeCell ref="E7:I7"/>
     <mergeCell ref="B8:D8"/>
     <mergeCell ref="B10:I10"/>
-    <mergeCell ref="B11:I11"/>
-    <mergeCell ref="B13:I13"/>
-    <mergeCell ref="B14:I14"/>
-    <mergeCell ref="C17:E17"/>
-    <mergeCell ref="G17:I17"/>
-    <mergeCell ref="C20:E20"/>
-    <mergeCell ref="G20:I20"/>
-    <mergeCell ref="B22:I22"/>
-    <mergeCell ref="C18:E18"/>
-    <mergeCell ref="C19:E19"/>
-    <mergeCell ref="G19:I19"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>